<commit_message>
residual block changed to bn-con-bn
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>69.90541955343514</v>
+        <v>73.99634758930016</v>
       </c>
       <c r="E1">
-        <v>72.7236385974107</v>
+        <v>81.15917896601891</v>
       </c>
       <c r="F1">
-        <v>74.32304610821046</v>
+        <v>81.2465081557779</v>
       </c>
       <c r="G1">
-        <v>46.82942097455713</v>
+        <v>50.48582899066636</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>86.90799788233782</v>
+        <v>82.64315965187087</v>
       </c>
       <c r="E2">
         <v>91.79104477611941</v>
       </c>
       <c r="F2">
-        <v>89.31515108405068</v>
+        <v>89.0788227794947</v>
       </c>
       <c r="G2">
-        <v>56.91668038649714</v>
+        <v>56.96652626645226</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>83.28470881708321</v>
+        <v>82.37175119075714</v>
       </c>
       <c r="E3">
-        <v>83.91877921828879</v>
+        <v>82.10526315789474</v>
       </c>
       <c r="F3">
-        <v>87.0536961178225</v>
+        <v>88.85717287867</v>
       </c>
       <c r="G3">
-        <v>57.26464480374861</v>
+        <v>58.34935759910164</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>66.28371338606318</v>
+        <v>65.99759979096662</v>
       </c>
       <c r="E4">
-        <v>71.7948717948718</v>
+        <v>89.58601855256981</v>
       </c>
       <c r="F4">
-        <v>69.89880328173655</v>
+        <v>84.44585712280185</v>
       </c>
       <c r="G4">
-        <v>47.94594812891905</v>
+        <v>59.50711060001895</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>63.35241424397741</v>
+        <v>83.38054610977025</v>
       </c>
       <c r="E5">
-        <v>80</v>
+        <v>93.33333333333333</v>
       </c>
       <c r="F5">
-        <v>79.9199631461546</v>
+        <v>92.13180261186042</v>
       </c>
       <c r="G5">
-        <v>49.52579693337044</v>
+        <v>61.80863502204452</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>46.9673665273143</v>
+        <v>60.34451962776261</v>
       </c>
       <c r="E6">
-        <v>55.00000000000001</v>
+        <v>70</v>
       </c>
       <c r="F6">
-        <v>53.39906930146743</v>
+        <v>69.46200917038148</v>
       </c>
       <c r="G6">
-        <v>23.72189081444856</v>
+        <v>30.90858859204694</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>74.99220566434828</v>
+        <v>82.77008847366228</v>
       </c>
       <c r="E7">
-        <v>78.91619107844573</v>
+        <v>73.68421052631578</v>
       </c>
       <c r="F7">
-        <v>79.57396200700995</v>
+        <v>77.83944508861406</v>
       </c>
       <c r="G7">
-        <v>47.19386882318395</v>
+        <v>43.55886154819326</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>74.0059039203754</v>
+        <v>63.65253892605208</v>
       </c>
       <c r="E8">
-        <v>50.36822191155986</v>
+        <v>51.58543628872329</v>
       </c>
       <c r="F8">
-        <v>65.96139158813698</v>
+        <v>62.15223808968322</v>
       </c>
       <c r="G8">
-        <v>41.81213570135151</v>
+        <v>34.63078129070227</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>63.44904598598144</v>
+        <v>70.81057694355933</v>
       </c>
       <c r="E9">
-        <v>70</v>
+        <v>97.18812509319491</v>
       </c>
       <c r="F9">
-        <v>69.46233233930502</v>
+        <v>86.00471750471749</v>
       </c>
       <c r="G9">
-        <v>50.25440220493775</v>
+        <v>58.15677100677099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
YoloV5 new head configuration
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>73.99634758930016</v>
+        <v>83.25813693486151</v>
       </c>
       <c r="E1">
-        <v>81.15917896601891</v>
+        <v>71.67677128301931</v>
       </c>
       <c r="F1">
-        <v>81.2465081557779</v>
+        <v>80.10421153793146</v>
       </c>
       <c r="G1">
-        <v>50.48582899066636</v>
+        <v>49.77323929997574</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>82.64315965187087</v>
+        <v>88.69064379680171</v>
       </c>
       <c r="E2">
-        <v>91.79104477611941</v>
+        <v>83.5820895522388</v>
       </c>
       <c r="F2">
-        <v>89.0788227794947</v>
+        <v>88.93408196366551</v>
       </c>
       <c r="G2">
-        <v>56.96652626645226</v>
+        <v>57.15146087056657</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>82.37175119075714</v>
+        <v>77.36234332043063</v>
       </c>
       <c r="E3">
-        <v>82.10526315789474</v>
+        <v>82.7399820993484</v>
       </c>
       <c r="F3">
-        <v>88.85717287867</v>
+        <v>87.49168007674703</v>
       </c>
       <c r="G3">
-        <v>58.34935759910164</v>
+        <v>56.59935659290447</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>65.99759979096662</v>
+        <v>71.847952275506</v>
       </c>
       <c r="E4">
-        <v>89.58601855256981</v>
+        <v>74.35897435897436</v>
       </c>
       <c r="F4">
-        <v>84.44585712280185</v>
+        <v>78.90054256799399</v>
       </c>
       <c r="G4">
-        <v>59.50711060001895</v>
+        <v>54.77615803240615</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>83.38054610977025</v>
+        <v>85.6372827442285</v>
       </c>
       <c r="E5">
-        <v>93.33333333333333</v>
+        <v>73.33333333333333</v>
       </c>
       <c r="F5">
-        <v>92.13180261186042</v>
+        <v>87.97758469471823</v>
       </c>
       <c r="G5">
-        <v>61.80863502204452</v>
+        <v>56.22302412499841</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>60.34451962776261</v>
+        <v>76.01580307869507</v>
       </c>
       <c r="E6">
-        <v>70</v>
+        <v>63.45373046756322</v>
       </c>
       <c r="F6">
-        <v>69.46200917038148</v>
+        <v>66.82727256720689</v>
       </c>
       <c r="G6">
-        <v>30.90858859204694</v>
+        <v>32.79735102212972</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>82.77008847366228</v>
+        <v>85.23002923335929</v>
       </c>
       <c r="E7">
-        <v>73.68421052631578</v>
+        <v>63.1578947368421</v>
       </c>
       <c r="F7">
-        <v>77.83944508861406</v>
+        <v>82.6639771799408</v>
       </c>
       <c r="G7">
-        <v>43.55886154819326</v>
+        <v>46.55771347202847</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>63.65253892605208</v>
+        <v>81.28104102987085</v>
       </c>
       <c r="E8">
-        <v>51.58543628872329</v>
+        <v>52.94117647058824</v>
       </c>
       <c r="F8">
-        <v>62.15223808968322</v>
+        <v>62.68403347916787</v>
       </c>
       <c r="G8">
-        <v>34.63078129070227</v>
+        <v>36.31741651201629</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>70.81057694355933</v>
+        <v>100</v>
       </c>
       <c r="E9">
-        <v>97.18812509319491</v>
+        <v>79.84698924526595</v>
       </c>
       <c r="F9">
-        <v>86.00471750471749</v>
+        <v>85.35451977401129</v>
       </c>
       <c r="G9">
-        <v>58.15677100677099</v>
+        <v>57.7634337727558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
stable autoencoder using mnist data set
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>83.25813693486151</v>
+        <v>0.6365460719280274</v>
       </c>
       <c r="E1">
-        <v>71.67677128301931</v>
+        <v>5.096915102979979</v>
       </c>
       <c r="F1">
-        <v>80.10421153793146</v>
+        <v>0.1237739816780862</v>
       </c>
       <c r="G1">
-        <v>49.77323929997574</v>
+        <v>0.01896930699493486</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>88.69064379680171</v>
+        <v>0.9257594155407242</v>
       </c>
       <c r="E2">
-        <v>83.5820895522388</v>
+        <v>6.716417910447761</v>
       </c>
       <c r="F2">
-        <v>88.93408196366551</v>
+        <v>0.1560913856018062</v>
       </c>
       <c r="G2">
-        <v>57.15146087056657</v>
+        <v>0.03299834600909928</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>77.36234332043063</v>
+        <v>1.222686689997595</v>
       </c>
       <c r="E3">
-        <v>82.7399820993484</v>
+        <v>9.473684210526317</v>
       </c>
       <c r="F3">
-        <v>87.49168007674703</v>
+        <v>0.2684382142522298</v>
       </c>
       <c r="G3">
-        <v>56.59935659290447</v>
+        <v>0.03825234534431345</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>71.847952275506</v>
+        <v>0.06895546953592396</v>
       </c>
       <c r="E4">
-        <v>74.35897435897436</v>
+        <v>12.82051282051282</v>
       </c>
       <c r="F4">
-        <v>78.90054256799399</v>
+        <v>0.1571457784186893</v>
       </c>
       <c r="G4">
-        <v>54.77615803240615</v>
+        <v>0.02542506513314081</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>85.6372827442285</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>73.33333333333333</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>87.97758469471823</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>56.22302412499841</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>76.01580307869507</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>63.45373046756322</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>66.82727256720689</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>32.79735102212972</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>85.23002923335929</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>63.1578947368421</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>82.6639771799408</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>46.55771347202847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>81.28104102987085</v>
+        <v>2.874967000349976</v>
       </c>
       <c r="E8">
-        <v>52.94117647058824</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="F8">
-        <v>62.68403347916787</v>
+        <v>0.3729488452576417</v>
       </c>
       <c r="G8">
-        <v>36.31741651201629</v>
+        <v>0.03729488452576417</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>79.84698924526595</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>85.35451977401129</v>
+        <v>0.03556762989432234</v>
       </c>
       <c r="G9">
-        <v>57.7634337727558</v>
+        <v>0.01778381494716117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
master branch code updated
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>0.6365460719280274</v>
+        <v>68.17709991409968</v>
       </c>
       <c r="E1">
-        <v>5.096915102979979</v>
+        <v>72.14331646379448</v>
       </c>
       <c r="F1">
-        <v>0.1237739816780862</v>
+        <v>73.05243123138962</v>
       </c>
       <c r="G1">
-        <v>0.01896930699493486</v>
+        <v>42.88452623217619</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>0.9257594155407242</v>
+        <v>80.53147070105067</v>
       </c>
       <c r="E2">
-        <v>6.716417910447761</v>
+        <v>85.07462686567165</v>
       </c>
       <c r="F2">
-        <v>0.1560913856018062</v>
+        <v>85.60849030440302</v>
       </c>
       <c r="G2">
-        <v>0.03299834600909928</v>
+        <v>54.64641705294696</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>1.222686689997595</v>
+        <v>74.45049886913807</v>
       </c>
       <c r="E3">
-        <v>9.473684210526317</v>
+        <v>79.75264751006495</v>
       </c>
       <c r="F3">
-        <v>0.2684382142522298</v>
+        <v>80.44781521322891</v>
       </c>
       <c r="G3">
-        <v>0.03825234534431345</v>
+        <v>51.88594645843765</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>0.06895546953592396</v>
+        <v>59.52251958002392</v>
       </c>
       <c r="E4">
-        <v>12.82051282051282</v>
+        <v>71.64330274225603</v>
       </c>
       <c r="F4">
-        <v>0.1571457784186893</v>
+        <v>67.56447684451997</v>
       </c>
       <c r="G4">
-        <v>0.02542506513314081</v>
+        <v>45.05974583798825</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>69.38626482441448</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>76.66666666666667</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>83.40054994615512</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>47.64263970045284</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>71.4383148407932</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>55.00000000000001</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>61.14347932559139</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>23.55577734366527</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>72.66193058683237</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>68.42105263157895</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>75.06667551845975</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>38.00636203072422</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>2.874967000349976</v>
+        <v>74.61180520482702</v>
       </c>
       <c r="E8">
-        <v>11.76470588235294</v>
+        <v>70.58823529411765</v>
       </c>
       <c r="F8">
-        <v>0.3729488452576417</v>
+        <v>68.25713015681517</v>
       </c>
       <c r="G8">
-        <v>0.03729488452576417</v>
+        <v>40.72825938824338</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>42.81399470571772</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F9">
-        <v>0.03556762989432234</v>
+        <v>62.93083254194365</v>
       </c>
       <c r="G9">
-        <v>0.01778381494716117</v>
+        <v>41.55106204495092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
autoencoder + denoising working completely
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>0.6365460719280274</v>
+        <v>74.68892899475621</v>
       </c>
       <c r="E1">
-        <v>5.096915102979979</v>
+        <v>65.53000827120312</v>
       </c>
       <c r="F1">
-        <v>0.1237739816780862</v>
+        <v>74.74188805366863</v>
       </c>
       <c r="G1">
-        <v>0.01896930699493486</v>
+        <v>44.57478156206889</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>0.9257594155407242</v>
+        <v>82.18830467834425</v>
       </c>
       <c r="E2">
-        <v>6.716417910447761</v>
+        <v>86.08869682104951</v>
       </c>
       <c r="F2">
-        <v>0.1560913856018062</v>
+        <v>89.70325366658092</v>
       </c>
       <c r="G2">
-        <v>0.03299834600909928</v>
+        <v>57.58147059387897</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>1.222686689997595</v>
+        <v>77.10845606866206</v>
       </c>
       <c r="E3">
-        <v>9.473684210526317</v>
+        <v>78.94736842105263</v>
       </c>
       <c r="F3">
-        <v>0.2684382142522298</v>
+        <v>85.41844990062607</v>
       </c>
       <c r="G3">
-        <v>0.03825234534431345</v>
+        <v>55.9817849898298</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>0.06895546953592396</v>
+        <v>61.84084445161264</v>
       </c>
       <c r="E4">
-        <v>12.82051282051282</v>
+        <v>69.23076923076923</v>
       </c>
       <c r="F4">
-        <v>0.1571457784186893</v>
+        <v>71.91099027191366</v>
       </c>
       <c r="G4">
-        <v>0.02542506513314081</v>
+        <v>47.45809110621789</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>89.88957635196672</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>59.30065022912257</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>80.11025142721257</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>48.12989550573491</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>90.86068932359662</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>66.20471320557093</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>30.50546296633821</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>69.69683544783204</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>73.68421052631578</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>81.93583847496714</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>41.95455089912883</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>2.874967000349976</v>
+        <v>57.10337272535252</v>
       </c>
       <c r="E8">
-        <v>11.76470588235294</v>
+        <v>46.98837094131527</v>
       </c>
       <c r="F8">
-        <v>0.3729488452576417</v>
+        <v>56.48564413547995</v>
       </c>
       <c r="G8">
-        <v>0.03729488452576417</v>
+        <v>30.37860614754947</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>68.82335291068271</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="F9">
-        <v>0.03556762989432234</v>
+        <v>66.16596334699783</v>
       </c>
       <c r="G9">
-        <v>0.01778381494716117</v>
+        <v>44.60839028787305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fso traffic surveillance multimodal fusion modified
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>74.68892899475621</v>
+        <v>74.09959141782021</v>
       </c>
       <c r="E1">
-        <v>65.53000827120312</v>
+        <v>69.7495764717564</v>
       </c>
       <c r="F1">
-        <v>74.74188805366863</v>
+        <v>75.60851697382053</v>
       </c>
       <c r="G1">
-        <v>44.57478156206889</v>
+        <v>46.65899651072027</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>82.18830467834425</v>
+        <v>81.28255498987505</v>
       </c>
       <c r="E2">
-        <v>86.08869682104951</v>
+        <v>87.31343283582089</v>
       </c>
       <c r="F2">
-        <v>89.70325366658092</v>
+        <v>88.0257118391762</v>
       </c>
       <c r="G2">
-        <v>57.58147059387897</v>
+        <v>54.59505829322553</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>77.10845606866206</v>
+        <v>76.52897860845974</v>
       </c>
       <c r="E3">
-        <v>78.94736842105263</v>
+        <v>78.9402611679718</v>
       </c>
       <c r="F3">
-        <v>85.41844990062607</v>
+        <v>83.52244808428784</v>
       </c>
       <c r="G3">
-        <v>55.9817849898298</v>
+        <v>55.22708804312752</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>61.84084445161264</v>
+        <v>64.09806044595639</v>
       </c>
       <c r="E4">
-        <v>69.23076923076923</v>
+        <v>77.83593418714574</v>
       </c>
       <c r="F4">
-        <v>71.91099027191366</v>
+        <v>75.37359958084393</v>
       </c>
       <c r="G4">
-        <v>47.45809110621789</v>
+        <v>53.86404028268929</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>89.88957635196672</v>
+        <v>78.07097819933374</v>
       </c>
       <c r="E5">
-        <v>59.30065022912257</v>
+        <v>70</v>
       </c>
       <c r="F5">
-        <v>80.11025142721257</v>
+        <v>80.44693264884725</v>
       </c>
       <c r="G5">
-        <v>48.12989550573491</v>
+        <v>49.89970152683711</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>90.86068932359662</v>
+        <v>59.88556718271083</v>
       </c>
       <c r="E6">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F6">
-        <v>66.20471320557093</v>
+        <v>55.83447857831657</v>
       </c>
       <c r="G6">
-        <v>30.50546296633821</v>
+        <v>30.19692758414841</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>69.69683544783204</v>
+        <v>85.85760571164558</v>
       </c>
       <c r="E7">
-        <v>73.68421052631578</v>
+        <v>63.1578947368421</v>
       </c>
       <c r="F7">
-        <v>81.93583847496714</v>
+        <v>83.7635312299786</v>
       </c>
       <c r="G7">
-        <v>41.95455089912883</v>
+        <v>44.94315103634182</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>57.10337272535252</v>
+        <v>69.90412165577962</v>
       </c>
       <c r="E8">
-        <v>46.98837094131527</v>
+        <v>52.94117647058824</v>
       </c>
       <c r="F8">
-        <v>56.48564413547995</v>
+        <v>57.69113535565742</v>
       </c>
       <c r="G8">
-        <v>30.37860614754947</v>
+        <v>33.37770958004413</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>68.82335291068271</v>
+        <v>77.16886454880066</v>
       </c>
       <c r="E9">
-        <v>60</v>
+        <v>67.80791237568233</v>
       </c>
       <c r="F9">
-        <v>66.16596334699783</v>
+        <v>80.21029847345636</v>
       </c>
       <c r="G9">
-        <v>44.60839028787305</v>
+        <v>51.16829573934838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wdsr with cbam implemented
</commit_message>
<xml_diff>
--- a/hello.xlsx
+++ b/hello.xlsx
@@ -389,16 +389,16 @@
         <v>364</v>
       </c>
       <c r="D1">
-        <v>74.09959141782021</v>
+        <v>72.19546185756005</v>
       </c>
       <c r="E1">
-        <v>69.7495764717564</v>
+        <v>68.03466573986856</v>
       </c>
       <c r="F1">
-        <v>75.60851697382053</v>
+        <v>75.31799530475331</v>
       </c>
       <c r="G1">
-        <v>46.65899651072027</v>
+        <v>46.98604995041558</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -412,16 +412,16 @@
         <v>134</v>
       </c>
       <c r="D2">
-        <v>81.28255498987505</v>
+        <v>87.03647529732335</v>
       </c>
       <c r="E2">
-        <v>87.31343283582089</v>
+        <v>88.05970149253731</v>
       </c>
       <c r="F2">
-        <v>88.0257118391762</v>
+        <v>91.72929683277631</v>
       </c>
       <c r="G2">
-        <v>54.59505829322553</v>
+        <v>60.27230927466055</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -435,16 +435,16 @@
         <v>95</v>
       </c>
       <c r="D3">
-        <v>76.52897860845974</v>
+        <v>83.79597989968964</v>
       </c>
       <c r="E3">
-        <v>78.9402611679718</v>
+        <v>81.05263157894737</v>
       </c>
       <c r="F3">
-        <v>83.52244808428784</v>
+        <v>86.80992373668454</v>
       </c>
       <c r="G3">
-        <v>55.22708804312752</v>
+        <v>56.55069923331617</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -458,16 +458,16 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>64.09806044595639</v>
+        <v>67.61082822216818</v>
       </c>
       <c r="E4">
-        <v>77.83593418714574</v>
+        <v>71.7948717948718</v>
       </c>
       <c r="F4">
-        <v>75.37359958084393</v>
+        <v>74.01012561155727</v>
       </c>
       <c r="G4">
-        <v>53.86404028268929</v>
+        <v>49.44491841088518</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -481,16 +481,16 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>78.07097819933374</v>
+        <v>86.9070804769934</v>
       </c>
       <c r="E5">
-        <v>70</v>
+        <v>66.38869690398516</v>
       </c>
       <c r="F5">
-        <v>80.44693264884725</v>
+        <v>82.37378585618382</v>
       </c>
       <c r="G5">
-        <v>49.89970152683711</v>
+        <v>50.39777090646778</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -504,16 +504,16 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>59.88556718271083</v>
+        <v>51.54262008714885</v>
       </c>
       <c r="E6">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="F6">
-        <v>55.83447857831657</v>
+        <v>51.21796290830382</v>
       </c>
       <c r="G6">
-        <v>30.19692758414841</v>
+        <v>23.40386746250383</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -527,16 +527,16 @@
         <v>19</v>
       </c>
       <c r="D7">
-        <v>85.85760571164558</v>
+        <v>74.16122199734127</v>
       </c>
       <c r="E7">
         <v>63.1578947368421</v>
       </c>
       <c r="F7">
-        <v>83.7635312299786</v>
+        <v>73.79197351085223</v>
       </c>
       <c r="G7">
-        <v>44.94315103634182</v>
+        <v>39.58647961306428</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -550,16 +550,16 @@
         <v>17</v>
       </c>
       <c r="D8">
-        <v>69.90412165577962</v>
+        <v>62.26611875163128</v>
       </c>
       <c r="E8">
-        <v>52.94117647058824</v>
+        <v>58.82352941176471</v>
       </c>
       <c r="F8">
-        <v>57.69113535565742</v>
+        <v>61.88774439574727</v>
       </c>
       <c r="G8">
-        <v>33.37770958004413</v>
+        <v>34.38301464031504</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -573,16 +573,16 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>77.16886454880066</v>
+        <v>64.24337012818449</v>
       </c>
       <c r="E9">
-        <v>67.80791237568233</v>
+        <v>80</v>
       </c>
       <c r="F9">
-        <v>80.21029847345636</v>
+        <v>80.72314958592133</v>
       </c>
       <c r="G9">
-        <v>51.16829573934838</v>
+        <v>61.8493400621118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>